<commit_message>
updated graphs and sql queries
</commit_message>
<xml_diff>
--- a/Charts/Avg price by state and year.xlsx
+++ b/Charts/Avg price by state and year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6880ced5148aa379/Desktop/Courses/UIUC/CS513 - Theory and Practice of Data Cleaning/Project/new_repo/CS513-Project/Charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{7E353394-5609-4F3B-9849-C94B3DA26D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{599DD934-3023-44A8-B700-2DA338EC91C8}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{7E353394-5609-4F3B-9849-C94B3DA26D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A51415C-EE37-4027-B2B7-75CA5E84A2A7}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15720" tabRatio="705" activeTab="1" xr2:uid="{36D508FB-902B-4F2E-8352-EA750F384C07}"/>
   </bookViews>
@@ -14943,6 +14943,7 @@
         <c:axId val="1895057584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2020"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -19790,7 +19791,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Menu Price by Year in NY (RAW)</a:t>
+              <a:t> Menu Price by Year in NY (CLEANED)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -41519,8 +41520,8 @@
   </sheetPr>
   <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>